<commit_message>
organized Economy class in methods and used Round in Trip calculation
</commit_message>
<xml_diff>
--- a/SupportingDocuments/Planets.xlsx
+++ b/SupportingDocuments/Planets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MSSA Cohort 6\Assignments\Week 4\SpaceTracker Pair Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MSSA Cohort 6\Assignments\Week 4\SpaceTracker Pair Project\MSSA_Exercise_4A\SupportingDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37948EA1-9BED-415C-B8B5-4A411C028DA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E97F164-E366-4294-81C0-7918D98B3D05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="3690" xr2:uid="{B0797FC1-E02C-483F-996F-2D7DB2AADDE4}"/>
   </bookViews>
@@ -203,8 +203,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -377,15 +377,15 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -600,7 +600,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC9158C2-4A13-42A8-A7CF-0BAA2192DF91}" type="CELLRANGE">
+                    <a:fld id="{D4B7CAE3-FF19-4D15-88F3-E8F5E0960AB4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -639,7 +639,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{32375B11-8C23-449F-943B-A25E89FB1CDA}" type="CELLRANGE">
+                    <a:fld id="{E0D90B69-AA8E-411B-9BD3-B44B92B75FE0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -672,7 +672,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D18025A-F998-4089-94D7-9C708440B88F}" type="CELLRANGE">
+                    <a:fld id="{2C223062-8643-46BD-B5FF-6D882FED02E9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -712,7 +712,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C31ACB45-4117-4FA6-978B-3F4621C5A2EE}" type="CELLRANGE">
+                    <a:fld id="{3ACAB916-F48A-40D4-9397-4EF54D984576}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -751,7 +751,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7127104F-1B15-4A7B-8B98-894AEA9B05F0}" type="CELLRANGE">
+                    <a:fld id="{E68F53C9-04E8-49E8-877A-E4F08D95B1A3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -784,7 +784,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{020636D9-C1B5-48F1-9291-F9503BBAE610}" type="CELLRANGE">
+                    <a:fld id="{CC9625B4-E6F0-4DA2-98C2-BE8D911E90D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -818,7 +818,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC377DB2-1158-4EC9-BDE6-A257029AB534}" type="CELLRANGE">
+                    <a:fld id="{8D6F4213-DC00-43D7-BCBC-CE069C092D2C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -852,7 +852,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4E76A1E-35FA-4209-B35E-ECB827C700FE}" type="CELLRANGE">
+                    <a:fld id="{45675C53-A29A-4EC4-A38B-0E67DB588871}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -892,7 +892,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{52890F99-A1A8-46D9-9CA7-0A757FF9DAB8}" type="CELLRANGE">
+                    <a:fld id="{5C562AEB-40B9-4495-8870-6EEB19E229AF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -925,7 +925,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE27FC47-96CD-4A14-AB9E-A15F736F5E88}" type="CELLRANGE">
+                    <a:fld id="{B467BB49-5725-4D42-9410-1B014D5D6B4D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -959,7 +959,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3459150-A430-4DE8-964E-6F8C4F044D1D}" type="CELLRANGE">
+                    <a:fld id="{2F5A5F56-DAF1-428A-9798-ECB1478521C3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -993,7 +993,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F4DAFAD0-AEAB-445A-A91C-179CBE1D499B}" type="CELLRANGE">
+                    <a:fld id="{294ECE22-B649-4160-A0CF-7A1B62F5533E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1027,7 +1027,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EE3F39DA-043B-4ED8-8ABA-49130E0EEAF7}" type="CELLRANGE">
+                    <a:fld id="{5C2CDA10-4C90-480C-9D34-83CBE4294E3B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1061,7 +1061,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF4F4D72-C370-40B9-9651-17708465CA4D}" type="CELLRANGE">
+                    <a:fld id="{A5A046EA-753C-4ED9-A5F4-8710766A6BD4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2358,7 +2358,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2527,7 +2527,7 @@
         <v>-12.802500789158705</v>
       </c>
       <c r="L5" s="25">
-        <f t="shared" ref="L5:L17" si="5">SQRT(POWER(J5-J4,2)+POWER(K5-K4,2))</f>
+        <f t="shared" ref="L5:L16" si="5">SQRT(POWER(J5-J4,2)+POWER(K5-K4,2))</f>
         <v>24.905019954615756</v>
       </c>
     </row>
@@ -3818,7 +3818,7 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C16" sqref="C16:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
added menu logic sheet to excel (wip)
</commit_message>
<xml_diff>
--- a/SupportingDocuments/Planets.xlsx
+++ b/SupportingDocuments/Planets.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MSSA Cohort 6\Assignments\Week 4\SpaceTracker Pair Project\MSSA_Exercise_4A\SupportingDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E97F164-E366-4294-81C0-7918D98B3D05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC97393F-A505-4D99-BEC7-96C14FD8CBFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="3690" xr2:uid="{B0797FC1-E02C-483F-996F-2D7DB2AADDE4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="3690" firstSheet="1" activeTab="2" xr2:uid="{B0797FC1-E02C-483F-996F-2D7DB2AADDE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planets" sheetId="1" r:id="rId1"/>
     <sheet name="Ores" sheetId="2" r:id="rId2"/>
     <sheet name="Economy" sheetId="3" r:id="rId3"/>
+    <sheet name="Menu Logic" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="79">
   <si>
     <t>distance LY</t>
   </si>
@@ -195,6 +196,81 @@
   </si>
   <si>
     <t>distance to earth</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>Dependencies</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Up/Down</t>
+  </si>
+  <si>
+    <t>None (Go Back to Main)</t>
+  </si>
+  <si>
+    <t>Start/Main</t>
+  </si>
+  <si>
+    <t>Enter/Esc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MenuOnlySelection() </t>
+  </si>
+  <si>
+    <t>MenuOnly</t>
+  </si>
+  <si>
+    <t>Continue (not implement)</t>
+  </si>
+  <si>
+    <t>New (needs to clear)</t>
+  </si>
+  <si>
+    <t>Quit (not implement)</t>
+  </si>
+  <si>
+    <t>Travel</t>
+  </si>
+  <si>
+    <t>Trade</t>
+  </si>
+  <si>
+    <t>In Game (new)</t>
+  </si>
+  <si>
+    <t>Fuel</t>
+  </si>
+  <si>
+    <t>Main Menu (start)</t>
+  </si>
+  <si>
+    <t>FullSelectionInput</t>
+  </si>
+  <si>
+    <t>Actions (Type enum)</t>
+  </si>
+  <si>
+    <t>M/R/T</t>
+  </si>
+  <si>
+    <t>MainMenu</t>
+  </si>
+  <si>
+    <t>Game State (decide action)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travel </t>
+  </si>
+  <si>
+    <t>Display planet</t>
   </si>
 </sst>
 </file>
@@ -345,7 +421,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -390,6 +466,7 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -600,7 +677,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4B7CAE3-FF19-4D15-88F3-E8F5E0960AB4}" type="CELLRANGE">
+                    <a:fld id="{A4F555F8-458D-4B90-826D-D7CFC7ADD2B4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -639,7 +716,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E0D90B69-AA8E-411B-9BD3-B44B92B75FE0}" type="CELLRANGE">
+                    <a:fld id="{CB98AA89-CCE7-414A-A244-377810359314}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -672,7 +749,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C223062-8643-46BD-B5FF-6D882FED02E9}" type="CELLRANGE">
+                    <a:fld id="{44379BA7-0D76-4A84-BA86-1F44D4FEBFC1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -712,7 +789,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3ACAB916-F48A-40D4-9397-4EF54D984576}" type="CELLRANGE">
+                    <a:fld id="{9BA7FF63-C9ED-48B7-805C-04D213062396}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -751,7 +828,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E68F53C9-04E8-49E8-877A-E4F08D95B1A3}" type="CELLRANGE">
+                    <a:fld id="{BD45B0EF-5AFE-47FE-BCCD-0C49E83ED90F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -784,7 +861,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC9625B4-E6F0-4DA2-98C2-BE8D911E90D3}" type="CELLRANGE">
+                    <a:fld id="{D2538B67-61E7-41EF-AD3C-5D191A9E98E9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -818,7 +895,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8D6F4213-DC00-43D7-BCBC-CE069C092D2C}" type="CELLRANGE">
+                    <a:fld id="{6F189801-516C-4626-8CFF-58692E763C5B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -852,7 +929,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{45675C53-A29A-4EC4-A38B-0E67DB588871}" type="CELLRANGE">
+                    <a:fld id="{B3001E64-8053-4AF8-A2D8-873C8D31DFAD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -892,7 +969,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C562AEB-40B9-4495-8870-6EEB19E229AF}" type="CELLRANGE">
+                    <a:fld id="{562B12FC-DEF1-4FA9-BB91-B797553550EA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -925,7 +1002,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B467BB49-5725-4D42-9410-1B014D5D6B4D}" type="CELLRANGE">
+                    <a:fld id="{44E51867-ED06-4949-AEFF-A3F7DF3B1F8D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -959,7 +1036,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F5A5F56-DAF1-428A-9798-ECB1478521C3}" type="CELLRANGE">
+                    <a:fld id="{6C15D795-018E-48ED-AC49-BD186E6EF475}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -993,7 +1070,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{294ECE22-B649-4160-A0CF-7A1B62F5533E}" type="CELLRANGE">
+                    <a:fld id="{F477D822-E37B-434E-A33F-149ECA7FFFD6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1027,7 +1104,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C2CDA10-4C90-480C-9D34-83CBE4294E3B}" type="CELLRANGE">
+                    <a:fld id="{15949591-5CBF-411B-AB85-76A3F3FB0FAD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1061,7 +1138,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5A046EA-753C-4ED9-A5F4-8710766A6BD4}" type="CELLRANGE">
+                    <a:fld id="{62551432-43D4-478E-87F4-4D5A8FF141A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2357,7 +2434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D1EBD2-C93E-4ACD-B3D5-764B3CC2D9EA}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+    <sheetView zoomScale="84" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -3817,8 +3894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77A70D4-1CA2-45FF-A5BD-2EA7477DBD43}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C25"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5139,4 +5216,127 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3FA1AA-58D9-4FEE-8DB5-FFA22B27030E}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.3984375" customWidth="1"/>
+    <col min="3" max="3" width="26.86328125" customWidth="1"/>
+    <col min="4" max="5" width="27.6640625" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.06640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>